<commit_message>
Clean Code for Submission
</commit_message>
<xml_diff>
--- a/Results_binary_recall.xlsx
+++ b/Results_binary_recall.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/14ac161be9f08974/Dokumente/GitHub/Machine-Learning-Case/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_6906C7A991E6E8BF891C87653AEE69FBC13C59E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B91B717-35C3-4A7E-A233-5A05565E653D}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="2040" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -88,11 +82,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,31 +92,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -155,32 +135,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -222,7 +192,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,27 +224,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,24 +258,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,200 +433,197 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2">
         <v>0.7874396135265701</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.82222222222222219</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.82233333333333325</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.82222222222222219</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0.82186825949892151</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="E2">
+        <v>0.8222222222222222</v>
+      </c>
+      <c r="F2">
+        <v>0.8223333333333332</v>
+      </c>
+      <c r="G2">
+        <v>0.8222222222222222</v>
+      </c>
+      <c r="H2">
+        <v>0.8218682594989215</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2">
         <v>2</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.75551684088269455</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="D3">
+        <v>0.7555168408826946</v>
+      </c>
+      <c r="E3">
         <v>0.8</v>
       </c>
-      <c r="E3" s="2">
-        <v>0.80370370370370381</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="F3">
+        <v>0.8037037037037038</v>
+      </c>
+      <c r="G3">
         <v>0.8</v>
       </c>
-      <c r="G3" s="2">
-        <v>0.79819004524886883</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3">
+        <v>0.7981900452488688</v>
+      </c>
+      <c r="I3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3">
         <v>10</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:12">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.87922705314009664</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4">
+        <v>0.8792270531400966</v>
+      </c>
+      <c r="E4">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="F4">
         <v>0.84</v>
       </c>
-      <c r="F4" s="2">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.83142100617828774</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="G4">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="H4">
+        <v>0.8314210061782877</v>
+      </c>
+      <c r="I4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5">
         <v>7</v>
       </c>
-      <c r="C5" s="2">
-        <v>0.83569492837785531</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.83630800611932699</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.83218448427121183</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="D5">
+        <v>0.8356949283778553</v>
+      </c>
+      <c r="E5">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="F5">
+        <v>0.836308006119327</v>
+      </c>
+      <c r="G5">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="H5">
+        <v>0.8321844842712118</v>
+      </c>
+      <c r="I5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5">
         <v>2</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>